<commit_message>
Charts and results exportation automaticaly
</commit_message>
<xml_diff>
--- a/_results/results.xlsx
+++ b/_results/results.xlsx
@@ -1,69 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Data e Hora</t>
-  </si>
-  <si>
-    <t>Dataframe</t>
-  </si>
-  <si>
-    <t>MAE</t>
-  </si>
-  <si>
-    <t>MSE</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>df_90_emmvi</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,18 +71,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,51 +438,274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>date_and_time</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dataframe_and_method</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>result_mae</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>result_mse</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>result_r2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>result_accuracy</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>status_mae</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status_mse</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>status_r2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>status_accurancy</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>min_range_mae</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>min_range_mse</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>min_range_r2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>min_range_accuracy</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>max_range_mae</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>max_range_mse</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>max_range_r2</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>max_range_accuracy</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>correlation_original_90</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>correlation_original_imputed</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>correlation_90_imputed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45079.57950555556</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>df_90_emmvi</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1.648068669527897</v>
+      </c>
+      <c r="D2" t="n">
+        <v>56.17167381974249</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8387993983120767</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9055793991416309</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>-18.70722292145952</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-349.9601894331804</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O2" t="n">
+        <v>18.70722292145952</v>
+      </c>
+      <c r="P2" t="n">
+        <v>349.9601894331804</v>
+      </c>
+      <c r="Q2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.9176343220749243</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2">
-        <v>45078.95473646216</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1.658593909666871</v>
-      </c>
-      <c r="D2">
-        <v>57.2395245880899</v>
-      </c>
-      <c r="E2">
-        <v>0.8357348966751322</v>
-      </c>
-      <c r="F2">
-        <v>0.08974358974358974</v>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>45079.58150693149</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>df_90_emmvi</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1.648068669527897</v>
+      </c>
+      <c r="D3" t="n">
+        <v>56.17167381974249</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8387993983120767</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9055793991416309</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Good performance!</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>-18.70722292145952</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-349.9601894331804</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="O3" t="n">
+        <v>18.70722292145952</v>
+      </c>
+      <c r="P3" t="n">
+        <v>349.9601894331804</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.9176343220749243</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>